<commit_message>
Updated the cathie changes
</commit_message>
<xml_diff>
--- a/TIARA_CAARS_AUTO_v1.0.1/TIARA_CAARS_AUTO_v1.0.1/PolicyNumbers.xlsx
+++ b/TIARA_CAARS_AUTO_v1.0.1/TIARA_CAARS_AUTO_v1.0.1/PolicyNumbers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUBRAMAS\OneDrive - AA PLC\UiPath\TIARA_CAARS_AUTO_v1.0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUBRAMAS\OneDrive - AA PLC\UiPath\Uipath_Projects\RPA\TIARA_CAARS_AUTO_v1.0.1\TIARA_CAARS_AUTO_v1.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C6C1D0C5-7391-4E08-B3FD-64E897AD8BA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{748760AF-279C-489B-9638-2E5FC1BF5073}"/>
@@ -400,7 +400,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>